<commit_message>
Merged UI plan in single excel file
</commit_message>
<xml_diff>
--- a/MyFirstApp.xlsx
+++ b/MyFirstApp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://targetonline-my.sharepoint.com/personal/anitha_r_target_com/Documents/ryse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z004m39/Documents/Development/learningresources-api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{B92EC707-6EE6-AB46-BA36-A60023899EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EFE37B3-D3BD-194E-8ED4-AAFCD938F138}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C11ECA-E9B5-0248-8AED-FA1535DDBE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="129">
   <si>
     <t>Day Number</t>
   </si>
@@ -269,13 +269,250 @@
   </si>
   <si>
     <t>Practise Day</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>UI Fundamentals</t>
+  </si>
+  <si>
+    <t>Basic crash course on HTML</t>
+  </si>
+  <si>
+    <t>Basic understanding on HTML/CSS and Javascript to get started on UI @ Target</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=N8YMl4Ezp4g&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=1</t>
+  </si>
+  <si>
+    <t>Basic crash course on CSS</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Icf5D3fEKbM&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=2</t>
+  </si>
+  <si>
+    <t>Basic crash course on JS and ES6</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XIOLqoPHCJ4&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=5</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>UI @ Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Able to create an Praxis app. Make it up and run locally. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intro to Praxis:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Getting started with Praxis Auth: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://web.microsoftstream.com/video/805d6bd7-d025-4cf1-b577-dc6ca4e648b8</t>
+    </r>
+  </si>
+  <si>
+    <t>Intro to Preaxis Framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create an app via Praxis framework </t>
+  </si>
+  <si>
+    <t>Getting Started with Enterprise Auth</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Introduce to React concepts</t>
+  </si>
+  <si>
+    <t>Hands on with react concepts (creating/exporting react components)</t>
+  </si>
+  <si>
+    <t>Basic idea on react components and react state.</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/react-fundamentals-update/table-of-contents</t>
+  </si>
+  <si>
+    <t>Functional and Class components.</t>
+  </si>
+  <si>
+    <t>Overview on React State and setState();</t>
+  </si>
+  <si>
+    <t>day 4</t>
+  </si>
+  <si>
+    <t>API calls with axios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consume a dummy API call using axios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn axios and consume sample API to render the data in UI. Commit the code to git. </t>
+  </si>
+  <si>
+    <t>https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx#part-7-posts-part-1
+https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx#part-8-posts-part-2
+https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx#part-9-post-details-part-1
+https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx#part-10-post-details-part-2
+https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx#part-11-post-details-part-3</t>
+  </si>
+  <si>
+    <t>Render the response from API call.</t>
+  </si>
+  <si>
+    <t>Day 5:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intro to Context API </t>
+  </si>
+  <si>
+    <t>State management through Context API.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hands on state management with Context API </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 6: </t>
+  </si>
+  <si>
+    <t>React Hooks</t>
+  </si>
+  <si>
+    <t>Intro to react hooks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement frequent used react hooks and implement praxis auth module </t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/using-react-hooks/table-of-contents</t>
+  </si>
+  <si>
+    <t>Different kind of hooks.</t>
+  </si>
+  <si>
+    <t>Implement Praxis auth module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 7: </t>
+  </si>
+  <si>
+    <t>Use case impl.</t>
+  </si>
+  <si>
+    <t>Start Implementation of use case components.</t>
+  </si>
+  <si>
+    <t>Create new praxis app for use case with Auth module. Commit to git.</t>
+  </si>
+  <si>
+    <t>https://targetonline.sharepoint.com/sites/Ryse/SitePages/Praxis-Self-Guided-Training.aspx</t>
+  </si>
+  <si>
+    <t>Integrate actual use case API using axios and render in UI.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">Complete UI channel: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://app.pluralsight.com/channels/details/ae86845a-02ce-4cdd-b921-c70ed7fea21a</t>
+    </r>
+  </si>
+  <si>
+    <t>Learning outcome</t>
+  </si>
+  <si>
+    <t>Learning Resource</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Design a simple HTML page with form fields and on click of Save button add them to a table grid in the same HTML web page. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Check-in the same to individual git repo.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Create a praxis app from Target's Praxis framework.
+2. Integrate Auth module to the app for successful authentication.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,16 +528,102 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -308,15 +631,242 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -631,7 +1181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD769F7-84F1-304B-BAF2-61CA75D9842C}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
@@ -986,12 +1536,356 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88729696-F004-9343-BD95-51CC42ED1E18}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="78.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="39"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="33"/>
+    </row>
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="C7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="39"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
+      <c r="C8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="40"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="33"/>
+    </row>
+    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="40"/>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" display="https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00" xr:uid="{7DA8ACA2-12C6-9D4A-AE49-FA78F117ED54}"/>
+    <hyperlink ref="E26" r:id="rId2" xr:uid="{DAFC891F-9857-994A-BD18-3FAE967F11FC}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{EB80BC5E-568A-2C47-911C-6748935DD28F}"/>
+    <hyperlink ref="E22" r:id="rId4" xr:uid="{229C7A2E-809E-604F-9B31-37BD8DA5312B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add links to UI path
</commit_message>
<xml_diff>
--- a/MyFirstApp.xlsx
+++ b/MyFirstApp.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://targetonline-my.sharepoint.com/personal/anitha_r_target_com/Documents/ryse/MyFirstAPI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Z004M39/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{2B9EF4C2-F320-8D49-B694-FD3562F201FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17BACC00-09DA-994C-8D6A-801FB9B8CF30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02609E7-0C28-C64A-8887-5FFF260D7993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
     <sheet name="UI" sheetId="2" r:id="rId2"/>
     <sheet name="Workshops" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="151">
   <si>
     <t>Day Number</t>
   </si>
@@ -272,21 +273,12 @@
     <t>Basic understanding on HTML/CSS and Javascript to get started on UI @ Target</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=N8YMl4Ezp4g&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=1</t>
-  </si>
-  <si>
     <t>Basic crash course on CSS</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=Icf5D3fEKbM&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=2</t>
-  </si>
-  <si>
     <t>Basic crash course on JS and ES6</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=XIOLqoPHCJ4&amp;list=PLC3y8-rFHvwhuX4qGvFx-wPy_MEi6Jdp7&amp;index=5</t>
-  </si>
-  <si>
     <t>Day 2</t>
   </si>
   <si>
@@ -294,55 +286,6 @@
   </si>
   <si>
     <t xml:space="preserve">Able to create an Praxis app. Make it up and run locally. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Intro to Praxis:</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Getting started with Praxis Auth: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="14"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://web.microsoftstream.com/video/805d6bd7-d025-4cf1-b577-dc6ca4e648b8</t>
-    </r>
   </si>
   <si>
     <t>Intro to Preaxis Framework</t>
@@ -553,12 +496,91 @@
   <si>
     <t>Add variables as mentioned in ReadMe</t>
   </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>Weekly Goal (23rd Feb - 4th Mar.)</t>
+  </si>
+  <si>
+    <t>Workshops completed:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jira board link : </t>
+  </si>
+  <si>
+    <t>https://jira.target.com/secure/RapidBoard.jspa?rapidView=8699</t>
+  </si>
+  <si>
+    <t>Create Rest API (GET/PUT/POST)</t>
+  </si>
+  <si>
+    <t>Connecting to DB</t>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/channels/details/ae86845a-02ce-4cdd-b921-c70ed7fea21a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Intro to Praxis:</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Getting started with Praxis Auth: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="16"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://web.microsoftstream.com/video/805d6bd7-d025-4cf1-b577-dc6ca4e648b8</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -605,23 +627,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -636,8 +641,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,8 +705,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -800,12 +855,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -814,9 +895,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -842,21 +920,42 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -881,34 +980,41 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1228,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD769F7-84F1-304B-BAF2-61CA75D9842C}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1280,7 +1386,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1290,8 +1396,8 @@
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>125</v>
+      <c r="E4" s="18" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1345,7 +1451,7 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1358,7 +1464,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1366,7 +1472,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1406,7 +1512,7 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1463,7 +1569,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1523,7 +1629,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1556,7 +1662,7 @@
         <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1580,10 +1686,10 @@
         <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1591,7 +1697,7 @@
         <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1602,10 +1708,10 @@
         <v>73</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E50" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1620,37 +1726,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88729696-F004-9343-BD95-51CC42ED1E18}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="78.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.5" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="17" t="s">
+      <c r="D1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1664,294 +1770,272 @@
       <c r="C2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="52" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="33"/>
+    </row>
+    <row r="4" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="27"/>
-    </row>
-    <row r="4" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="27"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="29"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="29"/>
+        <v>84</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="35"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="E12" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="9" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="B15" s="11" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="5" t="s">
+      <c r="D16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="E16" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="B15" s="12" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="302" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="13" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="B18" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="13" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="26"/>
-    </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B21" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="5" t="s">
+      <c r="D22" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="E22" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="B21" s="9" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="5" t="s">
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="B25" s="8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="5" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" ht="44" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="36"/>
-    </row>
-    <row r="24" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5" t="s">
+      <c r="D26" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="36"/>
-    </row>
-    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="E26" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="9" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="44" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="5" t="s">
+      <c r="D27" s="14"/>
+      <c r="E27" s="22"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="36"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="40"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A29:D30"/>
+  <mergeCells count="15">
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="D16:D17"/>
@@ -1961,12 +2045,19 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="E5:E8"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A29:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" display="https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00" xr:uid="{7DA8ACA2-12C6-9D4A-AE49-FA78F117ED54}"/>
     <hyperlink ref="E26" r:id="rId2" xr:uid="{DAFC891F-9857-994A-BD18-3FAE967F11FC}"/>
     <hyperlink ref="E12" r:id="rId3" xr:uid="{EB80BC5E-568A-2C47-911C-6748935DD28F}"/>
     <hyperlink ref="E22" r:id="rId4" xr:uid="{229C7A2E-809E-604F-9B31-37BD8DA5312B}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{A50C10D5-2FDC-9A40-9388-D2232DFF2CAB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1977,7 +2068,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+      <selection activeCell="B1" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1988,37 +2079,147 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4833FF-3F38-1A42-A9B1-E7B53C90F794}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="42"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="43"/>
+    </row>
+    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="45"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A13" r:id="rId1" xr:uid="{EE7D94DB-32D0-A140-95F8-5043276B8EC9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Corrected Java Pluralsight to specific course instead of path
</commit_message>
<xml_diff>
--- a/MyFirstApp.xlsx
+++ b/MyFirstApp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Z004M39/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://targetonline-my.sharepoint.com/personal/anitha_r_target_com/Documents/ryse/MyFirstAPI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02609E7-0C28-C64A-8887-5FFF260D7993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0DA8A77-82CD-B547-89CC-14702CECE74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
+    <workbookView xWindow="100" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{E40319C9-4210-CB41-94C4-B59EAEFA7522}"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="1" r:id="rId1"/>
@@ -438,9 +438,6 @@
   <si>
     <t>1. Create a praxis app from Target's Praxis framework.
 2. Integrate Auth module to the app for successful authentication.</t>
-  </si>
-  <si>
-    <t>https://app.pluralsight.com/paths/skill/java-language-fundamentals</t>
   </si>
   <si>
     <t>https://app.pluralsight.com/library/courses/creating-first-spring-boot-application/table-of-contents</t>
@@ -574,6 +571,9 @@
       </rPr>
       <t>https://web.microsoftstream.com/video/805d6bd7-d025-4cf1-b577-dc6ca4e648b8</t>
     </r>
+  </si>
+  <si>
+    <t>https://app.pluralsight.com/library/courses/getting-started-programming-java/table-of-contents</t>
   </si>
 </sst>
 </file>
@@ -920,101 +920,101 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1334,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD769F7-84F1-304B-BAF2-61CA75D9842C}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,7 +1386,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1397,7 +1397,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1451,7 +1451,7 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1464,7 +1464,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -1472,7 +1472,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1512,7 +1512,7 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1662,7 +1662,7 @@
         <v>65</v>
       </c>
       <c r="E42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1686,10 +1686,10 @@
         <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1697,7 +1697,7 @@
         <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1708,16 +1708,13 @@
         <v>73</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{0A18566D-7BD5-E546-A0AC-D09E03438A14}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1726,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88729696-F004-9343-BD95-51CC42ED1E18}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -1770,13 +1767,13 @@
       <c r="C2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="36" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1786,9 +1783,9 @@
       <c r="C3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="33"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
@@ -1796,9 +1793,9 @@
       <c r="C4" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="33"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1810,13 +1807,13 @@
       <c r="C5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="55" t="s">
-        <v>150</v>
-      </c>
-      <c r="F5" s="34" t="s">
+      <c r="E5" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1826,25 +1823,25 @@
       <c r="C6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="35"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="35"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.2">
       <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -1865,7 +1862,7 @@
       <c r="D12" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="30" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1876,7 +1873,7 @@
         <v>91</v>
       </c>
       <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -1885,7 +1882,7 @@
         <v>92</v>
       </c>
       <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
+      <c r="E14" s="31"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -1903,10 +1900,10 @@
       <c r="C16" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="34" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1916,8 +1913,8 @@
       <c r="C17" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="35"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
@@ -1935,7 +1932,7 @@
       <c r="C19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="32" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1945,7 +1942,7 @@
       <c r="C20" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="33"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
@@ -1963,10 +1960,10 @@
       <c r="C22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="47" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1976,8 +1973,8 @@
       <c r="C23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="48"/>
     </row>
     <row r="24" spans="1:5" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
@@ -1985,8 +1982,8 @@
       <c r="C24" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="48"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -2007,7 +2004,7 @@
       <c r="D26" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="57" t="s">
+      <c r="E26" s="47" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2018,24 +2015,29 @@
         <v>115</v>
       </c>
       <c r="D27" s="14"/>
-      <c r="E27" s="22"/>
+      <c r="E27" s="48"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="28"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A29:D30"/>
     <mergeCell ref="D12:D14"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="D16:D17"/>
@@ -2046,11 +2048,6 @@
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="E5:E8"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A29:D30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" display="https://web.microsoftstream.com/video/b691fabc-8dc9-4601-ae31-01b9afb44c00" xr:uid="{7DA8ACA2-12C6-9D4A-AE49-FA78F117ED54}"/>
@@ -2079,34 +2076,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
         <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
         <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
         <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2128,89 +2125,89 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:7" s="19" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="48" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="43"/>
+      <c r="B7" s="23"/>
     </row>
     <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="B12" s="57"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="45"/>
-    </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="51"/>
+      <c r="B13" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>